<commit_message>
se actualizó el escenario de ingreso de inventario, se agregó impresion de documentos, asigancion de series,informes
</commit_message>
<xml_diff>
--- a/web-automation-framework/src/main/resources/excel/BuscarOrden_WEB_DELIVERY.xlsx
+++ b/web-automation-framework/src/main/resources/excel/BuscarOrden_WEB_DELIVERY.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TC1</t>
   </si>
@@ -30,7 +30,19 @@
     <t>ORDEN</t>
   </si>
   <si>
-    <t>1004860</t>
+    <t>NUM_IMEI</t>
+  </si>
+  <si>
+    <t>NUM_SIMCARD</t>
+  </si>
+  <si>
+    <t>1005057</t>
+  </si>
+  <si>
+    <t>123600000007368</t>
+  </si>
+  <si>
+    <t>8954080008100062765</t>
   </si>
 </sst>
 </file>
@@ -82,12 +94,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -381,7 +390,7 @@
   <dimension ref="A1:Y71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,42 +401,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
     </row>
     <row r="2" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="2"/>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="T2" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
se actualizo el flujo de impresion de documentos
</commit_message>
<xml_diff>
--- a/web-automation-framework/src/main/resources/excel/BuscarOrden_WEB_DELIVERY.xlsx
+++ b/web-automation-framework/src/main/resources/excel/BuscarOrden_WEB_DELIVERY.xlsx
@@ -36,13 +36,13 @@
     <t>NUM_SIMCARD</t>
   </si>
   <si>
-    <t>1005057</t>
-  </si>
-  <si>
-    <t>123600000007368</t>
-  </si>
-  <si>
-    <t>8954080008100062765</t>
+    <t>1005069</t>
+  </si>
+  <si>
+    <t>8954080008100062856</t>
+  </si>
+  <si>
+    <t>123600000007459</t>
   </si>
 </sst>
 </file>
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y71"/>
+  <dimension ref="A1:Y54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,10 +440,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="T2" t="s">
         <v>1</v>
@@ -501,23 +501,6 @@
     <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://200.60.223.154/maximo/webclient/login/login2.jsp"/>

</xml_diff>